<commit_message>
regional tests data update
</commit_message>
<xml_diff>
--- a/data/states/mich-tests-06-21-2022.xlsx
+++ b/data/states/mich-tests-06-21-2022.xlsx
@@ -674,13 +674,13 @@
         <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>15189</v>
+        <v>15232</v>
       </c>
       <c r="D2" t="n">
-        <v>1459779</v>
+        <v>1463912</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="3">
@@ -691,13 +691,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D3" t="n">
-        <v>27006</v>
+        <v>27102</v>
       </c>
       <c r="E3" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="4">
@@ -708,13 +708,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>15470</v>
+        <v>15514</v>
       </c>
       <c r="D4" t="n">
-        <v>1486785</v>
+        <v>1491014</v>
       </c>
       <c r="E4" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="5">
@@ -725,13 +725,13 @@
         <v>6</v>
       </c>
       <c r="C5" t="n">
-        <v>11490</v>
+        <v>11513</v>
       </c>
       <c r="D5" t="n">
-        <v>1261528</v>
+        <v>1264054</v>
       </c>
       <c r="E5" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="6">
@@ -748,7 +748,7 @@
         <v>71146</v>
       </c>
       <c r="E6" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="7">
@@ -759,13 +759,13 @@
         <v>8</v>
       </c>
       <c r="C7" t="n">
-        <v>12138</v>
+        <v>12161</v>
       </c>
       <c r="D7" t="n">
-        <v>1332675</v>
+        <v>1335200</v>
       </c>
       <c r="E7" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="8">
@@ -776,13 +776,13 @@
         <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>204526</v>
+        <v>204840</v>
       </c>
       <c r="D8" t="n">
-        <v>1732082</v>
+        <v>1734741</v>
       </c>
       <c r="E8" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="9">
@@ -793,13 +793,13 @@
         <v>7</v>
       </c>
       <c r="C9" t="n">
-        <v>4268</v>
+        <v>4270</v>
       </c>
       <c r="D9" t="n">
-        <v>36145</v>
+        <v>36162</v>
       </c>
       <c r="E9" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="10">
@@ -810,13 +810,13 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>208794</v>
+        <v>209110</v>
       </c>
       <c r="D10" t="n">
-        <v>1768227</v>
+        <v>1770903</v>
       </c>
       <c r="E10" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="11">
@@ -827,13 +827,13 @@
         <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>48683</v>
+        <v>48855</v>
       </c>
       <c r="D11" t="n">
-        <v>1713888</v>
+        <v>1719944</v>
       </c>
       <c r="E11" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="12">
@@ -850,7 +850,7 @@
         <v>35487</v>
       </c>
       <c r="E12" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="13">
@@ -861,13 +861,13 @@
         <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>49691</v>
+        <v>49863</v>
       </c>
       <c r="D13" t="n">
-        <v>1749375</v>
+        <v>1755430</v>
       </c>
       <c r="E13" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="14">
@@ -878,13 +878,13 @@
         <v>6</v>
       </c>
       <c r="C14" t="n">
-        <v>38091</v>
+        <v>38221</v>
       </c>
       <c r="D14" t="n">
-        <v>1633125</v>
+        <v>1638698</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="15">
@@ -901,7 +901,7 @@
         <v>45104</v>
       </c>
       <c r="E15" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="16">
@@ -912,13 +912,13 @@
         <v>8</v>
       </c>
       <c r="C16" t="n">
-        <v>39143</v>
+        <v>39273</v>
       </c>
       <c r="D16" t="n">
-        <v>1678228</v>
+        <v>1683802</v>
       </c>
       <c r="E16" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="17">
@@ -929,13 +929,13 @@
         <v>6</v>
       </c>
       <c r="C17" t="n">
-        <v>34162</v>
+        <v>34286</v>
       </c>
       <c r="D17" t="n">
-        <v>2295371</v>
+        <v>2303702</v>
       </c>
       <c r="E17" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="18">
@@ -952,7 +952,7 @@
         <v>43069</v>
       </c>
       <c r="E18" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="19">
@@ -963,13 +963,13 @@
         <v>8</v>
       </c>
       <c r="C19" t="n">
-        <v>34803</v>
+        <v>34927</v>
       </c>
       <c r="D19" t="n">
-        <v>2338440</v>
+        <v>2346771</v>
       </c>
       <c r="E19" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="20">
@@ -977,16 +977,16 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C20" t="n">
-        <v>74</v>
+        <v>13368</v>
       </c>
       <c r="D20" t="n">
-        <v>9014</v>
+        <v>1628457</v>
       </c>
       <c r="E20" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="21">
@@ -994,16 +994,16 @@
         <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>13335</v>
+        <v>74</v>
       </c>
       <c r="D21" t="n">
-        <v>1624437</v>
+        <v>9014</v>
       </c>
       <c r="E21" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="22">
@@ -1014,13 +1014,13 @@
         <v>8</v>
       </c>
       <c r="C22" t="n">
-        <v>13409</v>
+        <v>13442</v>
       </c>
       <c r="D22" t="n">
-        <v>1633451</v>
+        <v>1637471</v>
       </c>
       <c r="E22" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="23">
@@ -1031,13 +1031,13 @@
         <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>98019</v>
+        <v>98166</v>
       </c>
       <c r="D23" t="n">
-        <v>1592510</v>
+        <v>1594898</v>
       </c>
       <c r="E23" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="24">
@@ -1054,7 +1054,7 @@
         <v>47149</v>
       </c>
       <c r="E24" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="25">
@@ -1065,13 +1065,13 @@
         <v>8</v>
       </c>
       <c r="C25" t="n">
-        <v>100921</v>
+        <v>101068</v>
       </c>
       <c r="D25" t="n">
-        <v>1639659</v>
+        <v>1642047</v>
       </c>
       <c r="E25" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="26">
@@ -1079,16 +1079,16 @@
         <v>16</v>
       </c>
       <c r="B26" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>8314</v>
+        <v>227458</v>
       </c>
       <c r="D26" t="n">
-        <v>80620</v>
+        <v>2205632</v>
       </c>
       <c r="E26" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="27">
@@ -1096,16 +1096,16 @@
         <v>16</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C27" t="n">
-        <v>227018</v>
+        <v>8315</v>
       </c>
       <c r="D27" t="n">
-        <v>2201365</v>
+        <v>80630</v>
       </c>
       <c r="E27" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="28">
@@ -1116,13 +1116,13 @@
         <v>8</v>
       </c>
       <c r="C28" t="n">
-        <v>235332</v>
+        <v>235773</v>
       </c>
       <c r="D28" t="n">
-        <v>2281985</v>
+        <v>2286261</v>
       </c>
       <c r="E28" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="29">
@@ -1133,13 +1133,13 @@
         <v>6</v>
       </c>
       <c r="C29" t="n">
-        <v>23162</v>
+        <v>23231</v>
       </c>
       <c r="D29" t="n">
-        <v>1303726</v>
+        <v>1307610</v>
       </c>
       <c r="E29" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="30">
@@ -1150,13 +1150,13 @@
         <v>7</v>
       </c>
       <c r="C30" t="n">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="D30" t="n">
-        <v>50490</v>
+        <v>50602</v>
       </c>
       <c r="E30" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="31">
@@ -1167,13 +1167,13 @@
         <v>8</v>
       </c>
       <c r="C31" t="n">
-        <v>24059</v>
+        <v>24130</v>
       </c>
       <c r="D31" t="n">
-        <v>1354216</v>
+        <v>1358212</v>
       </c>
       <c r="E31" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="32">
@@ -1184,13 +1184,13 @@
         <v>6</v>
       </c>
       <c r="C32" t="n">
-        <v>369795</v>
+        <v>370421</v>
       </c>
       <c r="D32" t="n">
-        <v>2410643</v>
+        <v>2414724</v>
       </c>
       <c r="E32" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="33">
@@ -1201,13 +1201,13 @@
         <v>7</v>
       </c>
       <c r="C33" t="n">
-        <v>8565</v>
+        <v>8569</v>
       </c>
       <c r="D33" t="n">
-        <v>55834</v>
+        <v>55860</v>
       </c>
       <c r="E33" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="34">
@@ -1218,13 +1218,13 @@
         <v>8</v>
       </c>
       <c r="C34" t="n">
-        <v>378360</v>
+        <v>378990</v>
       </c>
       <c r="D34" t="n">
-        <v>2466477</v>
+        <v>2470584</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="35">
@@ -1235,13 +1235,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="n">
-        <v>80667</v>
+        <v>80838</v>
       </c>
       <c r="D35" t="n">
-        <v>1853689</v>
+        <v>1857619</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="36">
@@ -1252,13 +1252,13 @@
         <v>7</v>
       </c>
       <c r="C36" t="n">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="D36" t="n">
-        <v>22750</v>
+        <v>22773</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="37">
@@ -1269,13 +1269,13 @@
         <v>8</v>
       </c>
       <c r="C37" t="n">
-        <v>81657</v>
+        <v>81829</v>
       </c>
       <c r="D37" t="n">
-        <v>1876439</v>
+        <v>1880392</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="38">
@@ -1286,13 +1286,13 @@
         <v>6</v>
       </c>
       <c r="C38" t="n">
-        <v>340437</v>
+        <v>341456</v>
       </c>
       <c r="D38" t="n">
-        <v>2537564</v>
+        <v>2545159</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="39">
@@ -1303,13 +1303,13 @@
         <v>7</v>
       </c>
       <c r="C39" t="n">
-        <v>2368</v>
+        <v>2371</v>
       </c>
       <c r="D39" t="n">
-        <v>17651</v>
+        <v>17673</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="40">
@@ -1320,13 +1320,13 @@
         <v>8</v>
       </c>
       <c r="C40" t="n">
-        <v>342805</v>
+        <v>343827</v>
       </c>
       <c r="D40" t="n">
-        <v>2555214</v>
+        <v>2562832</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="41">
@@ -1337,13 +1337,13 @@
         <v>6</v>
       </c>
       <c r="C41" t="n">
-        <v>65184</v>
+        <v>65306</v>
       </c>
       <c r="D41" t="n">
-        <v>1258694</v>
+        <v>1261050</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="42">
@@ -1360,7 +1360,7 @@
         <v>21704</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="43">
@@ -1371,13 +1371,13 @@
         <v>8</v>
       </c>
       <c r="C43" t="n">
-        <v>66308</v>
+        <v>66430</v>
       </c>
       <c r="D43" t="n">
-        <v>1280399</v>
+        <v>1282754</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="44">
@@ -1388,13 +1388,13 @@
         <v>6</v>
       </c>
       <c r="C44" t="n">
-        <v>41012</v>
+        <v>41271</v>
       </c>
       <c r="D44" t="n">
-        <v>1568756</v>
+        <v>1578664</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="45">
@@ -1405,13 +1405,13 @@
         <v>7</v>
       </c>
       <c r="C45" t="n">
-        <v>1357</v>
+        <v>1358</v>
       </c>
       <c r="D45" t="n">
-        <v>51907</v>
+        <v>51945</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="46">
@@ -1422,13 +1422,13 @@
         <v>8</v>
       </c>
       <c r="C46" t="n">
-        <v>42369</v>
+        <v>42629</v>
       </c>
       <c r="D46" t="n">
-        <v>1620663</v>
+        <v>1630609</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="47">
@@ -1439,13 +1439,13 @@
         <v>6</v>
       </c>
       <c r="C47" t="n">
-        <v>32194</v>
+        <v>32294</v>
       </c>
       <c r="D47" t="n">
-        <v>1273698</v>
+        <v>1277655</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="48">
@@ -1462,7 +1462,7 @@
         <v>32165</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="49">
@@ -1473,13 +1473,13 @@
         <v>8</v>
       </c>
       <c r="C49" t="n">
-        <v>33007</v>
+        <v>33107</v>
       </c>
       <c r="D49" t="n">
-        <v>1305863</v>
+        <v>1309820</v>
       </c>
       <c r="E49" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="50">
@@ -1487,16 +1487,16 @@
         <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C50" t="n">
-        <v>577</v>
+        <v>56550</v>
       </c>
       <c r="D50" t="n">
-        <v>15449</v>
+        <v>1514097</v>
       </c>
       <c r="E50" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="51">
@@ -1504,16 +1504,16 @@
         <v>24</v>
       </c>
       <c r="B51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C51" t="n">
-        <v>56286</v>
+        <v>577</v>
       </c>
       <c r="D51" t="n">
-        <v>1507028</v>
+        <v>15449</v>
       </c>
       <c r="E51" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="52">
@@ -1524,13 +1524,13 @@
         <v>8</v>
       </c>
       <c r="C52" t="n">
-        <v>56863</v>
+        <v>57127</v>
       </c>
       <c r="D52" t="n">
-        <v>1522477</v>
+        <v>1529546</v>
       </c>
       <c r="E52" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="53">
@@ -1541,13 +1541,13 @@
         <v>6</v>
       </c>
       <c r="C53" t="n">
-        <v>53998</v>
+        <v>54196</v>
       </c>
       <c r="D53" t="n">
-        <v>1744685</v>
+        <v>1751082</v>
       </c>
       <c r="E53" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="54">
@@ -1558,13 +1558,13 @@
         <v>7</v>
       </c>
       <c r="C54" t="n">
-        <v>1604</v>
+        <v>1606</v>
       </c>
       <c r="D54" t="n">
-        <v>51826</v>
+        <v>51890</v>
       </c>
       <c r="E54" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="55">
@@ -1575,13 +1575,13 @@
         <v>8</v>
       </c>
       <c r="C55" t="n">
-        <v>55602</v>
+        <v>55802</v>
       </c>
       <c r="D55" t="n">
-        <v>1796511</v>
+        <v>1802973</v>
       </c>
       <c r="E55" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="56">
@@ -1592,13 +1592,13 @@
         <v>6</v>
       </c>
       <c r="C56" t="n">
-        <v>101249</v>
+        <v>101428</v>
       </c>
       <c r="D56" t="n">
-        <v>1272052</v>
+        <v>1274301</v>
       </c>
       <c r="E56" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="57">
@@ -1609,13 +1609,13 @@
         <v>7</v>
       </c>
       <c r="C57" t="n">
-        <v>5723</v>
+        <v>5725</v>
       </c>
       <c r="D57" t="n">
-        <v>71902</v>
+        <v>71927</v>
       </c>
       <c r="E57" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="58">
@@ -1626,13 +1626,13 @@
         <v>8</v>
       </c>
       <c r="C58" t="n">
-        <v>106972</v>
+        <v>107153</v>
       </c>
       <c r="D58" t="n">
-        <v>1343954</v>
+        <v>1346228</v>
       </c>
       <c r="E58" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="59">
@@ -1643,11 +1643,11 @@
         <v>6</v>
       </c>
       <c r="C59" t="n">
-        <v>1064887</v>
+        <v>1065139</v>
       </c>
       <c r="D59"/>
       <c r="E59" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="60">
@@ -1658,11 +1658,11 @@
         <v>7</v>
       </c>
       <c r="C60" t="n">
-        <v>35768</v>
+        <v>35771</v>
       </c>
       <c r="D60"/>
       <c r="E60" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="61">
@@ -1673,11 +1673,11 @@
         <v>8</v>
       </c>
       <c r="C61" t="n">
-        <v>1100655</v>
+        <v>1100910</v>
       </c>
       <c r="D61"/>
       <c r="E61" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="62">
@@ -1685,16 +1685,16 @@
         <v>28</v>
       </c>
       <c r="B62" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C62" t="n">
-        <v>484</v>
+        <v>20685</v>
       </c>
       <c r="D62" t="n">
-        <v>34500</v>
+        <v>1474446</v>
       </c>
       <c r="E62" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="63">
@@ -1702,16 +1702,16 @@
         <v>28</v>
       </c>
       <c r="B63" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C63" t="n">
-        <v>20638</v>
+        <v>485</v>
       </c>
       <c r="D63" t="n">
-        <v>1471096</v>
+        <v>34571</v>
       </c>
       <c r="E63" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="64">
@@ -1722,13 +1722,13 @@
         <v>8</v>
       </c>
       <c r="C64" t="n">
-        <v>21122</v>
+        <v>21170</v>
       </c>
       <c r="D64" t="n">
-        <v>1505596</v>
+        <v>1509017</v>
       </c>
       <c r="E64" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="65">
@@ -1739,13 +1739,13 @@
         <v>6</v>
       </c>
       <c r="C65" t="n">
-        <v>72076</v>
+        <v>72243</v>
       </c>
       <c r="D65" t="n">
-        <v>2014196</v>
+        <v>2018863</v>
       </c>
       <c r="E65" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="66">
@@ -1756,13 +1756,13 @@
         <v>7</v>
       </c>
       <c r="C66" t="n">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="D66" t="n">
-        <v>34876</v>
+        <v>34932</v>
       </c>
       <c r="E66" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="67">
@@ -1773,13 +1773,13 @@
         <v>8</v>
       </c>
       <c r="C67" t="n">
-        <v>73324</v>
+        <v>73493</v>
       </c>
       <c r="D67" t="n">
-        <v>2049072</v>
+        <v>2053795</v>
       </c>
       <c r="E67" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="68">
@@ -1787,16 +1787,16 @@
         <v>30</v>
       </c>
       <c r="B68" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C68" t="n">
-        <v>36241</v>
+        <v>2254204</v>
       </c>
       <c r="D68" t="n">
-        <v>55772</v>
+        <v>3469052</v>
       </c>
       <c r="E68" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="69">
@@ -1804,16 +1804,16 @@
         <v>30</v>
       </c>
       <c r="B69" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C69" t="n">
-        <v>2244540</v>
+        <v>36265</v>
       </c>
       <c r="D69" t="n">
-        <v>3454180</v>
+        <v>55809</v>
       </c>
       <c r="E69" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="70">
@@ -1824,13 +1824,13 @@
         <v>8</v>
       </c>
       <c r="C70" t="n">
-        <v>2280781</v>
+        <v>2290469</v>
       </c>
       <c r="D70" t="n">
-        <v>3509952</v>
+        <v>3524861</v>
       </c>
       <c r="E70" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="71">
@@ -1841,13 +1841,13 @@
         <v>6</v>
       </c>
       <c r="C71" t="n">
-        <v>38964</v>
+        <v>39161</v>
       </c>
       <c r="D71" t="n">
-        <v>1543801</v>
+        <v>1551607</v>
       </c>
       <c r="E71" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="72">
@@ -1864,7 +1864,7 @@
         <v>9707</v>
       </c>
       <c r="E72" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="73">
@@ -1875,13 +1875,13 @@
         <v>8</v>
       </c>
       <c r="C73" t="n">
-        <v>39209</v>
+        <v>39406</v>
       </c>
       <c r="D73" t="n">
-        <v>1553508</v>
+        <v>1561314</v>
       </c>
       <c r="E73" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="74">
@@ -1892,13 +1892,13 @@
         <v>6</v>
       </c>
       <c r="C74" t="n">
-        <v>234132</v>
+        <v>234599</v>
       </c>
       <c r="D74" t="n">
-        <v>2123300</v>
+        <v>2127535</v>
       </c>
       <c r="E74" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="75">
@@ -1909,13 +1909,13 @@
         <v>7</v>
       </c>
       <c r="C75" t="n">
-        <v>8367</v>
+        <v>8371</v>
       </c>
       <c r="D75" t="n">
-        <v>75879</v>
+        <v>75915</v>
       </c>
       <c r="E75" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="76">
@@ -1926,13 +1926,13 @@
         <v>8</v>
       </c>
       <c r="C76" t="n">
-        <v>242499</v>
+        <v>242970</v>
       </c>
       <c r="D76" t="n">
-        <v>2199178</v>
+        <v>2203450</v>
       </c>
       <c r="E76" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="77">
@@ -1943,13 +1943,13 @@
         <v>6</v>
       </c>
       <c r="C77" t="n">
-        <v>57548</v>
+        <v>57688</v>
       </c>
       <c r="D77" t="n">
-        <v>1722221</v>
+        <v>1726410</v>
       </c>
       <c r="E77" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="78">
@@ -1966,7 +1966,7 @@
         <v>59794</v>
       </c>
       <c r="E78" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="79">
@@ -1977,13 +1977,13 @@
         <v>8</v>
       </c>
       <c r="C79" t="n">
-        <v>59546</v>
+        <v>59686</v>
       </c>
       <c r="D79" t="n">
-        <v>1782014</v>
+        <v>1786204</v>
       </c>
       <c r="E79" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="80">
@@ -1991,16 +1991,16 @@
         <v>34</v>
       </c>
       <c r="B80" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C80" t="n">
-        <v>27344</v>
+        <v>743867</v>
       </c>
       <c r="D80" t="n">
-        <v>67381</v>
+        <v>1833029</v>
       </c>
       <c r="E80" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="81">
@@ -2008,16 +2008,16 @@
         <v>34</v>
       </c>
       <c r="B81" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C81" t="n">
-        <v>742295</v>
+        <v>27348</v>
       </c>
       <c r="D81" t="n">
-        <v>1829155</v>
+        <v>67391</v>
       </c>
       <c r="E81" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="82">
@@ -2028,13 +2028,13 @@
         <v>8</v>
       </c>
       <c r="C82" t="n">
-        <v>769639</v>
+        <v>771215</v>
       </c>
       <c r="D82" t="n">
-        <v>1896536</v>
+        <v>1900420</v>
       </c>
       <c r="E82" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="83">
@@ -2045,13 +2045,13 @@
         <v>6</v>
       </c>
       <c r="C83" t="n">
-        <v>45404</v>
+        <v>45654</v>
       </c>
       <c r="D83" t="n">
-        <v>1784117</v>
+        <v>1793941</v>
       </c>
       <c r="E83" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="84">
@@ -2062,13 +2062,13 @@
         <v>7</v>
       </c>
       <c r="C84" t="n">
-        <v>1396</v>
+        <v>1397</v>
       </c>
       <c r="D84" t="n">
-        <v>54855</v>
+        <v>54894</v>
       </c>
       <c r="E84" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="85">
@@ -2079,13 +2079,13 @@
         <v>8</v>
       </c>
       <c r="C85" t="n">
-        <v>46800</v>
+        <v>47051</v>
       </c>
       <c r="D85" t="n">
-        <v>1838972</v>
+        <v>1848835</v>
       </c>
       <c r="E85" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="86">
@@ -2096,13 +2096,13 @@
         <v>6</v>
       </c>
       <c r="C86" t="n">
-        <v>32306</v>
+        <v>32435</v>
       </c>
       <c r="D86" t="n">
-        <v>2311699</v>
+        <v>2320930</v>
       </c>
       <c r="E86" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="87">
@@ -2119,7 +2119,7 @@
         <v>20894</v>
       </c>
       <c r="E87" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="88">
@@ -2130,13 +2130,13 @@
         <v>8</v>
       </c>
       <c r="C88" t="n">
-        <v>32598</v>
+        <v>32727</v>
       </c>
       <c r="D88" t="n">
-        <v>2332594</v>
+        <v>2341825</v>
       </c>
       <c r="E88" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="89">
@@ -2147,13 +2147,13 @@
         <v>6</v>
       </c>
       <c r="C89" t="n">
-        <v>159811</v>
+        <v>160281</v>
       </c>
       <c r="D89" t="n">
-        <v>1716773</v>
+        <v>1721822</v>
       </c>
       <c r="E89" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="90">
@@ -2164,13 +2164,13 @@
         <v>7</v>
       </c>
       <c r="C90" t="n">
-        <v>7995</v>
+        <v>7996</v>
       </c>
       <c r="D90" t="n">
-        <v>85886</v>
+        <v>85897</v>
       </c>
       <c r="E90" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="91">
@@ -2181,13 +2181,13 @@
         <v>8</v>
       </c>
       <c r="C91" t="n">
-        <v>167806</v>
+        <v>168277</v>
       </c>
       <c r="D91" t="n">
-        <v>1802660</v>
+        <v>1807720</v>
       </c>
       <c r="E91" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="92">
@@ -2198,13 +2198,13 @@
         <v>6</v>
       </c>
       <c r="C92" t="n">
-        <v>98309</v>
+        <v>98527</v>
       </c>
       <c r="D92" t="n">
-        <v>2414802</v>
+        <v>2420157</v>
       </c>
       <c r="E92" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="93">
@@ -2221,7 +2221,7 @@
         <v>37385</v>
       </c>
       <c r="E93" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="94">
@@ -2232,13 +2232,13 @@
         <v>8</v>
       </c>
       <c r="C94" t="n">
-        <v>99831</v>
+        <v>100049</v>
       </c>
       <c r="D94" t="n">
-        <v>2452187</v>
+        <v>2457542</v>
       </c>
       <c r="E94" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="95">
@@ -2246,16 +2246,16 @@
         <v>39</v>
       </c>
       <c r="B95" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C95" t="n">
-        <v>1717</v>
+        <v>80207</v>
       </c>
       <c r="D95" t="n">
-        <v>37649</v>
+        <v>1758733</v>
       </c>
       <c r="E95" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="96">
@@ -2263,16 +2263,16 @@
         <v>39</v>
       </c>
       <c r="B96" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C96" t="n">
-        <v>80067</v>
+        <v>1717</v>
       </c>
       <c r="D96" t="n">
-        <v>1755663</v>
+        <v>37649</v>
       </c>
       <c r="E96" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="97">
@@ -2283,13 +2283,13 @@
         <v>8</v>
       </c>
       <c r="C97" t="n">
-        <v>81784</v>
+        <v>81924</v>
       </c>
       <c r="D97" t="n">
-        <v>1793312</v>
+        <v>1796382</v>
       </c>
       <c r="E97" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="98">
@@ -2300,13 +2300,13 @@
         <v>6</v>
       </c>
       <c r="C98" t="n">
-        <v>81891</v>
+        <v>82038</v>
       </c>
       <c r="D98" t="n">
-        <v>2294894</v>
+        <v>2299014</v>
       </c>
       <c r="E98" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="99">
@@ -2323,7 +2323,7 @@
         <v>9836</v>
       </c>
       <c r="E99" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="100">
@@ -2334,13 +2334,13 @@
         <v>8</v>
       </c>
       <c r="C100" t="n">
-        <v>82242</v>
+        <v>82389</v>
       </c>
       <c r="D100" t="n">
-        <v>2304730</v>
+        <v>2308850</v>
       </c>
       <c r="E100" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="101">
@@ -2348,16 +2348,16 @@
         <v>41</v>
       </c>
       <c r="B101" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C101" t="n">
-        <v>1551</v>
+        <v>51073</v>
       </c>
       <c r="D101" t="n">
-        <v>50063</v>
+        <v>1648527</v>
       </c>
       <c r="E101" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="102">
@@ -2365,16 +2365,16 @@
         <v>41</v>
       </c>
       <c r="B102" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C102" t="n">
-        <v>50889</v>
+        <v>1557</v>
       </c>
       <c r="D102" t="n">
-        <v>1642587</v>
+        <v>50257</v>
       </c>
       <c r="E102" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="103">
@@ -2385,13 +2385,13 @@
         <v>8</v>
       </c>
       <c r="C103" t="n">
-        <v>52440</v>
+        <v>52630</v>
       </c>
       <c r="D103" t="n">
-        <v>1692650</v>
+        <v>1698783</v>
       </c>
       <c r="E103" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="104">
@@ -2399,16 +2399,16 @@
         <v>42</v>
       </c>
       <c r="B104" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C104" t="n">
-        <v>24417</v>
+        <v>644728</v>
       </c>
       <c r="D104" t="n">
-        <v>83504</v>
+        <v>2204907</v>
       </c>
       <c r="E104" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="105">
@@ -2416,16 +2416,16 @@
         <v>42</v>
       </c>
       <c r="B105" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C105" t="n">
-        <v>643454</v>
+        <v>24435</v>
       </c>
       <c r="D105" t="n">
-        <v>2200550</v>
+        <v>83565</v>
       </c>
       <c r="E105" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="106">
@@ -2436,13 +2436,13 @@
         <v>8</v>
       </c>
       <c r="C106" t="n">
-        <v>667871</v>
+        <v>669163</v>
       </c>
       <c r="D106" t="n">
-        <v>2284054</v>
+        <v>2288472</v>
       </c>
       <c r="E106" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="107">
@@ -2453,13 +2453,13 @@
         <v>6</v>
       </c>
       <c r="C107" t="n">
-        <v>133124</v>
+        <v>133317</v>
       </c>
       <c r="D107" t="n">
-        <v>2057653</v>
+        <v>2060637</v>
       </c>
       <c r="E107" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="108">
@@ -2470,13 +2470,13 @@
         <v>7</v>
       </c>
       <c r="C108" t="n">
-        <v>3338</v>
+        <v>3339</v>
       </c>
       <c r="D108" t="n">
-        <v>51594</v>
+        <v>51610</v>
       </c>
       <c r="E108" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="109">
@@ -2487,13 +2487,13 @@
         <v>8</v>
       </c>
       <c r="C109" t="n">
-        <v>136462</v>
+        <v>136656</v>
       </c>
       <c r="D109" t="n">
-        <v>2109248</v>
+        <v>2112246</v>
       </c>
       <c r="E109" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="110">
@@ -2504,13 +2504,13 @@
         <v>6</v>
       </c>
       <c r="C110" t="n">
-        <v>49538</v>
+        <v>49654</v>
       </c>
       <c r="D110" t="n">
-        <v>1971505</v>
+        <v>1976121</v>
       </c>
       <c r="E110" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="111">
@@ -2521,13 +2521,13 @@
         <v>7</v>
       </c>
       <c r="C111" t="n">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D111" t="n">
-        <v>34306</v>
+        <v>34346</v>
       </c>
       <c r="E111" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="112">
@@ -2538,13 +2538,13 @@
         <v>8</v>
       </c>
       <c r="C112" t="n">
-        <v>50400</v>
+        <v>50517</v>
       </c>
       <c r="D112" t="n">
-        <v>2005810</v>
+        <v>2010467</v>
       </c>
       <c r="E112" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="113">
@@ -2555,13 +2555,13 @@
         <v>6</v>
       </c>
       <c r="C113" t="n">
-        <v>34999</v>
+        <v>35092</v>
       </c>
       <c r="D113" t="n">
-        <v>3162751</v>
+        <v>3171155</v>
       </c>
       <c r="E113" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="114">
@@ -2578,7 +2578,7 @@
         <v>16718</v>
       </c>
       <c r="E114" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="115">
@@ -2589,13 +2589,13 @@
         <v>8</v>
       </c>
       <c r="C115" t="n">
-        <v>35184</v>
+        <v>35277</v>
       </c>
       <c r="D115" t="n">
-        <v>3179469</v>
+        <v>3187873</v>
       </c>
       <c r="E115" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="116">
@@ -2606,13 +2606,13 @@
         <v>6</v>
       </c>
       <c r="C116" t="n">
-        <v>126227</v>
+        <v>126487</v>
       </c>
       <c r="D116" t="n">
-        <v>1806546</v>
+        <v>1810267</v>
       </c>
       <c r="E116" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="117">
@@ -2629,7 +2629,7 @@
         <v>29168</v>
       </c>
       <c r="E117" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="118">
@@ -2640,13 +2640,13 @@
         <v>8</v>
       </c>
       <c r="C118" t="n">
-        <v>128265</v>
+        <v>128525</v>
       </c>
       <c r="D118" t="n">
-        <v>1835714</v>
+        <v>1839435</v>
       </c>
       <c r="E118" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="119">
@@ -2654,16 +2654,16 @@
         <v>47</v>
       </c>
       <c r="B119" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C119" t="n">
-        <v>5754</v>
+        <v>383588</v>
       </c>
       <c r="D119" t="n">
-        <v>36301</v>
+        <v>2419961</v>
       </c>
       <c r="E119" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="120">
@@ -2671,16 +2671,16 @@
         <v>47</v>
       </c>
       <c r="B120" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C120" t="n">
-        <v>382739</v>
+        <v>5755</v>
       </c>
       <c r="D120" t="n">
-        <v>2414605</v>
+        <v>36307</v>
       </c>
       <c r="E120" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="121">
@@ -2691,13 +2691,13 @@
         <v>8</v>
       </c>
       <c r="C121" t="n">
-        <v>388493</v>
+        <v>389343</v>
       </c>
       <c r="D121" t="n">
-        <v>2450905</v>
+        <v>2456268</v>
       </c>
       <c r="E121" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="122">
@@ -2708,13 +2708,13 @@
         <v>6</v>
       </c>
       <c r="C122" t="n">
-        <v>580547</v>
+        <v>581772</v>
       </c>
       <c r="D122" t="n">
-        <v>2190198</v>
+        <v>2194819</v>
       </c>
       <c r="E122" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="123">
@@ -2731,7 +2731,7 @@
         <v>31030</v>
       </c>
       <c r="E123" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="124">
@@ -2742,13 +2742,13 @@
         <v>8</v>
       </c>
       <c r="C124" t="n">
-        <v>588772</v>
+        <v>589997</v>
       </c>
       <c r="D124" t="n">
-        <v>2221228</v>
+        <v>2225849</v>
       </c>
       <c r="E124" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="125">
@@ -2759,13 +2759,13 @@
         <v>6</v>
       </c>
       <c r="C125" t="n">
-        <v>32310</v>
+        <v>32392</v>
       </c>
       <c r="D125" t="n">
-        <v>1791219</v>
+        <v>1795764</v>
       </c>
       <c r="E125" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="126">
@@ -2782,7 +2782,7 @@
         <v>54108</v>
       </c>
       <c r="E126" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="127">
@@ -2793,13 +2793,13 @@
         <v>8</v>
       </c>
       <c r="C127" t="n">
-        <v>33286</v>
+        <v>33368</v>
       </c>
       <c r="D127" t="n">
-        <v>1845327</v>
+        <v>1849872</v>
       </c>
       <c r="E127" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="128">
@@ -2810,13 +2810,13 @@
         <v>6</v>
       </c>
       <c r="C128" t="n">
-        <v>1594072</v>
+        <v>1596806</v>
       </c>
       <c r="D128" t="n">
-        <v>2426455</v>
+        <v>2430617</v>
       </c>
       <c r="E128" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="129">
@@ -2827,13 +2827,13 @@
         <v>7</v>
       </c>
       <c r="C129" t="n">
-        <v>57962</v>
+        <v>57982</v>
       </c>
       <c r="D129" t="n">
-        <v>88228</v>
+        <v>88259</v>
       </c>
       <c r="E129" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="130">
@@ -2844,13 +2844,13 @@
         <v>8</v>
       </c>
       <c r="C130" t="n">
-        <v>1652034</v>
+        <v>1654788</v>
       </c>
       <c r="D130" t="n">
-        <v>2514684</v>
+        <v>2518876</v>
       </c>
       <c r="E130" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="131">
@@ -2861,13 +2861,13 @@
         <v>6</v>
       </c>
       <c r="C131" t="n">
-        <v>4146</v>
+        <v>4157</v>
       </c>
       <c r="D131" t="n">
-        <v>1959357</v>
+        <v>1964556</v>
       </c>
       <c r="E131" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="132">
@@ -2884,7 +2884,7 @@
         <v>19849</v>
       </c>
       <c r="E132" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="133">
@@ -2895,13 +2895,13 @@
         <v>8</v>
       </c>
       <c r="C133" t="n">
-        <v>4188</v>
+        <v>4199</v>
       </c>
       <c r="D133" t="n">
-        <v>1979206</v>
+        <v>1984405</v>
       </c>
       <c r="E133" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="134">
@@ -2912,13 +2912,13 @@
         <v>6</v>
       </c>
       <c r="C134" t="n">
-        <v>18243</v>
+        <v>18284</v>
       </c>
       <c r="D134" t="n">
-        <v>1539104</v>
+        <v>1542563</v>
       </c>
       <c r="E134" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="135">
@@ -2935,7 +2935,7 @@
         <v>25816</v>
       </c>
       <c r="E135" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="136">
@@ -2946,13 +2946,13 @@
         <v>8</v>
       </c>
       <c r="C136" t="n">
-        <v>18549</v>
+        <v>18590</v>
       </c>
       <c r="D136" t="n">
-        <v>1564920</v>
+        <v>1568379</v>
       </c>
       <c r="E136" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="137">
@@ -2960,16 +2960,16 @@
         <v>53</v>
       </c>
       <c r="B137" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C137" t="n">
-        <v>5749</v>
+        <v>128711</v>
       </c>
       <c r="D137" t="n">
-        <v>65623</v>
+        <v>1469186</v>
       </c>
       <c r="E137" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="138">
@@ -2977,16 +2977,16 @@
         <v>53</v>
       </c>
       <c r="B138" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C138" t="n">
-        <v>128434</v>
+        <v>5753</v>
       </c>
       <c r="D138" t="n">
-        <v>1466024</v>
+        <v>65668</v>
       </c>
       <c r="E138" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="139">
@@ -2997,13 +2997,13 @@
         <v>8</v>
       </c>
       <c r="C139" t="n">
-        <v>134183</v>
+        <v>134464</v>
       </c>
       <c r="D139" t="n">
-        <v>1531647</v>
+        <v>1534855</v>
       </c>
       <c r="E139" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="140">
@@ -3014,13 +3014,13 @@
         <v>6</v>
       </c>
       <c r="C140" t="n">
-        <v>22947</v>
+        <v>23018</v>
       </c>
       <c r="D140" t="n">
-        <v>1054501</v>
+        <v>1057764</v>
       </c>
       <c r="E140" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="141">
@@ -3037,7 +3037,7 @@
         <v>61808</v>
       </c>
       <c r="E141" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="142">
@@ -3048,13 +3048,13 @@
         <v>8</v>
       </c>
       <c r="C142" t="n">
-        <v>24292</v>
+        <v>24363</v>
       </c>
       <c r="D142" t="n">
-        <v>1116309</v>
+        <v>1119572</v>
       </c>
       <c r="E142" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="143">
@@ -3065,13 +3065,13 @@
         <v>6</v>
       </c>
       <c r="C143" t="n">
-        <v>234511</v>
+        <v>235153</v>
       </c>
       <c r="D143" t="n">
-        <v>2382007</v>
+        <v>2388528</v>
       </c>
       <c r="E143" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="144">
@@ -3082,13 +3082,13 @@
         <v>7</v>
       </c>
       <c r="C144" t="n">
-        <v>3534</v>
+        <v>3535</v>
       </c>
       <c r="D144" t="n">
-        <v>35896</v>
+        <v>35906</v>
       </c>
       <c r="E144" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="145">
@@ -3099,13 +3099,13 @@
         <v>8</v>
       </c>
       <c r="C145" t="n">
-        <v>238045</v>
+        <v>238688</v>
       </c>
       <c r="D145" t="n">
-        <v>2417903</v>
+        <v>2424434</v>
       </c>
       <c r="E145" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="146">
@@ -3113,16 +3113,16 @@
         <v>56</v>
       </c>
       <c r="B146" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C146" t="n">
-        <v>11726</v>
+        <v>392983</v>
       </c>
       <c r="D146" t="n">
-        <v>61075</v>
+        <v>2046840</v>
       </c>
       <c r="E146" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="147">
@@ -3130,16 +3130,16 @@
         <v>56</v>
       </c>
       <c r="B147" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C147" t="n">
-        <v>392133</v>
+        <v>11731</v>
       </c>
       <c r="D147" t="n">
-        <v>2042413</v>
+        <v>61101</v>
       </c>
       <c r="E147" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="148">
@@ -3150,13 +3150,13 @@
         <v>8</v>
       </c>
       <c r="C148" t="n">
-        <v>403859</v>
+        <v>404714</v>
       </c>
       <c r="D148" t="n">
-        <v>2103487</v>
+        <v>2107940</v>
       </c>
       <c r="E148" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="149">
@@ -3167,13 +3167,13 @@
         <v>6</v>
       </c>
       <c r="C149" t="n">
-        <v>9440</v>
+        <v>9451</v>
       </c>
       <c r="D149" t="n">
-        <v>1515492</v>
+        <v>1517258</v>
       </c>
       <c r="E149" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="150">
@@ -3190,7 +3190,7 @@
         <v>7224</v>
       </c>
       <c r="E150" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="151">
@@ -3201,13 +3201,13 @@
         <v>8</v>
       </c>
       <c r="C151" t="n">
-        <v>9485</v>
+        <v>9496</v>
       </c>
       <c r="D151" t="n">
-        <v>1522716</v>
+        <v>1524482</v>
       </c>
       <c r="E151" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="152">
@@ -3218,13 +3218,13 @@
         <v>6</v>
       </c>
       <c r="C152" t="n">
-        <v>17487</v>
+        <v>17614</v>
       </c>
       <c r="D152" t="n">
-        <v>1619317</v>
+        <v>1631077</v>
       </c>
       <c r="E152" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="153">
@@ -3241,7 +3241,7 @@
         <v>20835</v>
       </c>
       <c r="E153" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="154">
@@ -3252,13 +3252,13 @@
         <v>8</v>
       </c>
       <c r="C154" t="n">
-        <v>17712</v>
+        <v>17839</v>
       </c>
       <c r="D154" t="n">
-        <v>1640152</v>
+        <v>1651912</v>
       </c>
       <c r="E154" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="155">
@@ -3269,13 +3269,13 @@
         <v>6</v>
       </c>
       <c r="C155" t="n">
-        <v>1872400</v>
+        <v>1877293</v>
       </c>
       <c r="D155" t="n">
-        <v>2142403</v>
+        <v>2148001</v>
       </c>
       <c r="E155" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="156">
@@ -3286,13 +3286,13 @@
         <v>7</v>
       </c>
       <c r="C156" t="n">
-        <v>93749</v>
+        <v>93809</v>
       </c>
       <c r="D156" t="n">
-        <v>107268</v>
+        <v>107336</v>
       </c>
       <c r="E156" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="157">
@@ -3303,13 +3303,13 @@
         <v>8</v>
       </c>
       <c r="C157" t="n">
-        <v>1966149</v>
+        <v>1971102</v>
       </c>
       <c r="D157" t="n">
-        <v>2249670</v>
+        <v>2255338</v>
       </c>
       <c r="E157" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="158">
@@ -3320,13 +3320,13 @@
         <v>6</v>
       </c>
       <c r="C158" t="n">
-        <v>35235</v>
+        <v>35320</v>
       </c>
       <c r="D158" t="n">
-        <v>1434767</v>
+        <v>1438228</v>
       </c>
       <c r="E158" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="159">
@@ -3343,7 +3343,7 @@
         <v>47764</v>
       </c>
       <c r="E159" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="160">
@@ -3354,13 +3354,13 @@
         <v>8</v>
       </c>
       <c r="C160" t="n">
-        <v>36408</v>
+        <v>36493</v>
       </c>
       <c r="D160" t="n">
-        <v>1482531</v>
+        <v>1485992</v>
       </c>
       <c r="E160" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="161">
@@ -3371,13 +3371,13 @@
         <v>6</v>
       </c>
       <c r="C161" t="n">
-        <v>195108</v>
+        <v>195381</v>
       </c>
       <c r="D161" t="n">
-        <v>2925201</v>
+        <v>2929294</v>
       </c>
       <c r="E161" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="162">
@@ -3388,13 +3388,13 @@
         <v>7</v>
       </c>
       <c r="C162" t="n">
-        <v>1771</v>
+        <v>1775</v>
       </c>
       <c r="D162" t="n">
-        <v>26552</v>
+        <v>26612</v>
       </c>
       <c r="E162" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="163">
@@ -3405,13 +3405,13 @@
         <v>8</v>
       </c>
       <c r="C163" t="n">
-        <v>196879</v>
+        <v>197156</v>
       </c>
       <c r="D163" t="n">
-        <v>2951753</v>
+        <v>2955906</v>
       </c>
       <c r="E163" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="164">
@@ -3422,13 +3422,13 @@
         <v>6</v>
       </c>
       <c r="C164" t="n">
-        <v>67340</v>
+        <v>67522</v>
       </c>
       <c r="D164" t="n">
-        <v>2310596</v>
+        <v>2316841</v>
       </c>
       <c r="E164" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="165">
@@ -3439,13 +3439,13 @@
         <v>7</v>
       </c>
       <c r="C165" t="n">
-        <v>1439</v>
+        <v>1440</v>
       </c>
       <c r="D165" t="n">
-        <v>49376</v>
+        <v>49410</v>
       </c>
       <c r="E165" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="166">
@@ -3456,13 +3456,13 @@
         <v>8</v>
       </c>
       <c r="C166" t="n">
-        <v>68779</v>
+        <v>68962</v>
       </c>
       <c r="D166" t="n">
-        <v>2359971</v>
+        <v>2366250</v>
       </c>
       <c r="E166" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="167">
@@ -3470,16 +3470,16 @@
         <v>63</v>
       </c>
       <c r="B167" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C167" t="n">
-        <v>1452</v>
+        <v>70705</v>
       </c>
       <c r="D167" t="n">
-        <v>33415</v>
+        <v>1627160</v>
       </c>
       <c r="E167" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="168">
@@ -3487,16 +3487,16 @@
         <v>63</v>
       </c>
       <c r="B168" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C168" t="n">
-        <v>70597</v>
+        <v>1453</v>
       </c>
       <c r="D168" t="n">
-        <v>1624675</v>
+        <v>33438</v>
       </c>
       <c r="E168" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="169">
@@ -3507,13 +3507,13 @@
         <v>8</v>
       </c>
       <c r="C169" t="n">
-        <v>72049</v>
+        <v>72158</v>
       </c>
       <c r="D169" t="n">
-        <v>1658090</v>
+        <v>1660599</v>
       </c>
       <c r="E169" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="170">
@@ -3524,13 +3524,13 @@
         <v>6</v>
       </c>
       <c r="C170" t="n">
-        <v>45617</v>
+        <v>45768</v>
       </c>
       <c r="D170" t="n">
-        <v>2002502</v>
+        <v>2009131</v>
       </c>
       <c r="E170" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="171">
@@ -3547,7 +3547,7 @@
         <v>11370</v>
       </c>
       <c r="E171" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="172">
@@ -3558,13 +3558,13 @@
         <v>8</v>
       </c>
       <c r="C172" t="n">
-        <v>45876</v>
+        <v>46027</v>
       </c>
       <c r="D172" t="n">
-        <v>2013872</v>
+        <v>2020500</v>
       </c>
       <c r="E172" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="173">
@@ -3575,13 +3575,13 @@
         <v>6</v>
       </c>
       <c r="C173" t="n">
-        <v>145510</v>
+        <v>145971</v>
       </c>
       <c r="D173" t="n">
-        <v>1749844</v>
+        <v>1755387</v>
       </c>
       <c r="E173" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="174">
@@ -3592,13 +3592,13 @@
         <v>7</v>
       </c>
       <c r="C174" t="n">
-        <v>8537</v>
+        <v>8541</v>
       </c>
       <c r="D174" t="n">
-        <v>102662</v>
+        <v>102711</v>
       </c>
       <c r="E174" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="175">
@@ -3609,13 +3609,13 @@
         <v>8</v>
       </c>
       <c r="C175" t="n">
-        <v>154047</v>
+        <v>154512</v>
       </c>
       <c r="D175" t="n">
-        <v>1852506</v>
+        <v>1858098</v>
       </c>
       <c r="E175" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="176">
@@ -3623,16 +3623,16 @@
         <v>66</v>
       </c>
       <c r="B176" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C176" t="n">
-        <v>845</v>
+        <v>19538</v>
       </c>
       <c r="D176" t="n">
-        <v>55894</v>
+        <v>1292367</v>
       </c>
       <c r="E176" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="177">
@@ -3640,16 +3640,16 @@
         <v>66</v>
       </c>
       <c r="B177" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C177" t="n">
-        <v>19474</v>
+        <v>845</v>
       </c>
       <c r="D177" t="n">
-        <v>1288133</v>
+        <v>55894</v>
       </c>
       <c r="E177" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="178">
@@ -3660,13 +3660,13 @@
         <v>8</v>
       </c>
       <c r="C178" t="n">
-        <v>20319</v>
+        <v>20383</v>
       </c>
       <c r="D178" t="n">
-        <v>1344027</v>
+        <v>1348260</v>
       </c>
       <c r="E178" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="179">
@@ -3674,16 +3674,16 @@
         <v>67</v>
       </c>
       <c r="B179" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C179" t="n">
-        <v>8623</v>
+        <v>294410</v>
       </c>
       <c r="D179" t="n">
-        <v>57296</v>
+        <v>1956213</v>
       </c>
       <c r="E179" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="180">
@@ -3691,16 +3691,16 @@
         <v>67</v>
       </c>
       <c r="B180" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C180" t="n">
-        <v>293620</v>
+        <v>8626</v>
       </c>
       <c r="D180" t="n">
-        <v>1950963</v>
+        <v>57316</v>
       </c>
       <c r="E180" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="181">
@@ -3711,13 +3711,13 @@
         <v>8</v>
       </c>
       <c r="C181" t="n">
-        <v>302243</v>
+        <v>303036</v>
       </c>
       <c r="D181" t="n">
-        <v>2008259</v>
+        <v>2013528</v>
       </c>
       <c r="E181" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="182">
@@ -3725,16 +3725,16 @@
         <v>68</v>
       </c>
       <c r="B182" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C182" t="n">
-        <v>3436</v>
+        <v>135903</v>
       </c>
       <c r="D182" t="n">
-        <v>53782</v>
+        <v>2127207</v>
       </c>
       <c r="E182" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="183">
@@ -3742,16 +3742,16 @@
         <v>68</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C183" t="n">
-        <v>135620</v>
+        <v>3442</v>
       </c>
       <c r="D183" t="n">
-        <v>2122777</v>
+        <v>53876</v>
       </c>
       <c r="E183" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="184">
@@ -3762,13 +3762,13 @@
         <v>8</v>
       </c>
       <c r="C184" t="n">
-        <v>139056</v>
+        <v>139345</v>
       </c>
       <c r="D184" t="n">
-        <v>2176559</v>
+        <v>2181083</v>
       </c>
       <c r="E184" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="185">
@@ -3779,13 +3779,13 @@
         <v>6</v>
       </c>
       <c r="C185" t="n">
-        <v>16736</v>
+        <v>16788</v>
       </c>
       <c r="D185" t="n">
-        <v>1794168</v>
+        <v>1799743</v>
       </c>
       <c r="E185" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="186">
@@ -3802,7 +3802,7 @@
         <v>59605</v>
       </c>
       <c r="E186" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="187">
@@ -3813,13 +3813,13 @@
         <v>8</v>
       </c>
       <c r="C187" t="n">
-        <v>17292</v>
+        <v>17344</v>
       </c>
       <c r="D187" t="n">
-        <v>1853774</v>
+        <v>1859348</v>
       </c>
       <c r="E187" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="188">
@@ -3830,13 +3830,13 @@
         <v>6</v>
       </c>
       <c r="C188" t="n">
-        <v>385428</v>
+        <v>386411</v>
       </c>
       <c r="D188" t="n">
-        <v>2220642</v>
+        <v>2226306</v>
       </c>
       <c r="E188" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="189">
@@ -3847,13 +3847,13 @@
         <v>7</v>
       </c>
       <c r="C189" t="n">
-        <v>5487</v>
+        <v>5491</v>
       </c>
       <c r="D189" t="n">
-        <v>31613</v>
+        <v>31636</v>
       </c>
       <c r="E189" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="190">
@@ -3864,13 +3864,13 @@
         <v>8</v>
       </c>
       <c r="C190" t="n">
-        <v>390915</v>
+        <v>391902</v>
       </c>
       <c r="D190" t="n">
-        <v>2252256</v>
+        <v>2257942</v>
       </c>
       <c r="E190" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="191">
@@ -3878,16 +3878,16 @@
         <v>71</v>
       </c>
       <c r="B191" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C191" t="n">
-        <v>2418</v>
+        <v>82154</v>
       </c>
       <c r="D191" t="n">
-        <v>49367</v>
+        <v>1677297</v>
       </c>
       <c r="E191" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="192">
@@ -3895,16 +3895,16 @@
         <v>71</v>
       </c>
       <c r="B192" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C192" t="n">
-        <v>82009</v>
+        <v>2419</v>
       </c>
       <c r="D192" t="n">
-        <v>1674336</v>
+        <v>49388</v>
       </c>
       <c r="E192" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="193">
@@ -3915,13 +3915,13 @@
         <v>8</v>
       </c>
       <c r="C193" t="n">
-        <v>84427</v>
+        <v>84573</v>
       </c>
       <c r="D193" t="n">
-        <v>1723704</v>
+        <v>1726684</v>
       </c>
       <c r="E193" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="194">
@@ -3932,13 +3932,13 @@
         <v>6</v>
       </c>
       <c r="C194" t="n">
-        <v>2931841</v>
+        <v>2940097</v>
       </c>
       <c r="D194" t="n">
-        <v>2331328</v>
+        <v>2337893</v>
       </c>
       <c r="E194" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="195">
@@ -3949,13 +3949,13 @@
         <v>7</v>
       </c>
       <c r="C195" t="n">
-        <v>161241</v>
+        <v>161359</v>
       </c>
       <c r="D195" t="n">
-        <v>128215</v>
+        <v>128309</v>
       </c>
       <c r="E195" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="196">
@@ -3966,13 +3966,13 @@
         <v>8</v>
       </c>
       <c r="C196" t="n">
-        <v>3093082</v>
+        <v>3101456</v>
       </c>
       <c r="D196" t="n">
-        <v>2459543</v>
+        <v>2466202</v>
       </c>
       <c r="E196" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="197">
@@ -3983,13 +3983,13 @@
         <v>6</v>
       </c>
       <c r="C197" t="n">
-        <v>60832</v>
+        <v>60984</v>
       </c>
       <c r="D197" t="n">
-        <v>2298409</v>
+        <v>2304152</v>
       </c>
       <c r="E197" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="198">
@@ -4000,13 +4000,13 @@
         <v>7</v>
       </c>
       <c r="C198" t="n">
-        <v>1328</v>
+        <v>1331</v>
       </c>
       <c r="D198" t="n">
-        <v>50176</v>
+        <v>50289</v>
       </c>
       <c r="E198" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="199">
@@ -4017,13 +4017,13 @@
         <v>8</v>
       </c>
       <c r="C199" t="n">
-        <v>62160</v>
+        <v>62315</v>
       </c>
       <c r="D199" t="n">
-        <v>2348585</v>
+        <v>2354441</v>
       </c>
       <c r="E199" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="200">
@@ -4034,13 +4034,13 @@
         <v>6</v>
       </c>
       <c r="C200" t="n">
-        <v>36248</v>
+        <v>36378</v>
       </c>
       <c r="D200" t="n">
-        <v>1726342</v>
+        <v>1732533</v>
       </c>
       <c r="E200" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="201">
@@ -4057,7 +4057,7 @@
         <v>35196</v>
       </c>
       <c r="E201" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="202">
@@ -4068,13 +4068,13 @@
         <v>8</v>
       </c>
       <c r="C202" t="n">
-        <v>36987</v>
+        <v>37117</v>
       </c>
       <c r="D202" t="n">
-        <v>1761537</v>
+        <v>1767729</v>
       </c>
       <c r="E202" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="203">
@@ -4085,13 +4085,13 @@
         <v>6</v>
       </c>
       <c r="C203" t="n">
-        <v>12134</v>
+        <v>12161</v>
       </c>
       <c r="D203" t="n">
-        <v>2121329</v>
+        <v>2126049</v>
       </c>
       <c r="E203" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="204">
@@ -4108,7 +4108,7 @@
         <v>12937</v>
       </c>
       <c r="E204" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="205">
@@ -4119,13 +4119,13 @@
         <v>8</v>
       </c>
       <c r="C205" t="n">
-        <v>12208</v>
+        <v>12235</v>
       </c>
       <c r="D205" t="n">
-        <v>2134266</v>
+        <v>2138986</v>
       </c>
       <c r="E205" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="206">
@@ -4136,13 +4136,13 @@
         <v>6</v>
       </c>
       <c r="C206" t="n">
-        <v>45234</v>
+        <v>45341</v>
       </c>
       <c r="D206" t="n">
-        <v>1928133</v>
+        <v>1932694</v>
       </c>
       <c r="E206" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="207">
@@ -4153,13 +4153,13 @@
         <v>7</v>
       </c>
       <c r="C207" t="n">
-        <v>1709</v>
+        <v>1710</v>
       </c>
       <c r="D207" t="n">
-        <v>72847</v>
+        <v>72890</v>
       </c>
       <c r="E207" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="208">
@@ -4170,13 +4170,13 @@
         <v>8</v>
       </c>
       <c r="C208" t="n">
-        <v>46943</v>
+        <v>47051</v>
       </c>
       <c r="D208" t="n">
-        <v>2000980</v>
+        <v>2005584</v>
       </c>
       <c r="E208" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="209">
@@ -4187,13 +4187,13 @@
         <v>6</v>
       </c>
       <c r="C209" t="n">
-        <v>10417</v>
+        <v>10446</v>
       </c>
       <c r="D209" t="n">
-        <v>1264046</v>
+        <v>1267565</v>
       </c>
       <c r="E209" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="210">
@@ -4210,7 +4210,7 @@
         <v>51935</v>
       </c>
       <c r="E210" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="211">
@@ -4221,13 +4221,13 @@
         <v>8</v>
       </c>
       <c r="C211" t="n">
-        <v>10845</v>
+        <v>10874</v>
       </c>
       <c r="D211" t="n">
-        <v>1315981</v>
+        <v>1319500</v>
       </c>
       <c r="E211" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="212">
@@ -4235,16 +4235,16 @@
         <v>78</v>
       </c>
       <c r="B212" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C212" t="n">
-        <v>1536</v>
+        <v>46075</v>
       </c>
       <c r="D212" t="n">
-        <v>62267</v>
+        <v>1867804</v>
       </c>
       <c r="E212" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="213">
@@ -4252,16 +4252,16 @@
         <v>78</v>
       </c>
       <c r="B213" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C213" t="n">
-        <v>45943</v>
+        <v>1539</v>
       </c>
       <c r="D213" t="n">
-        <v>1862453</v>
+        <v>62389</v>
       </c>
       <c r="E213" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="214">
@@ -4272,13 +4272,13 @@
         <v>8</v>
       </c>
       <c r="C214" t="n">
-        <v>47479</v>
+        <v>47614</v>
       </c>
       <c r="D214" t="n">
-        <v>1924720</v>
+        <v>1930193</v>
       </c>
       <c r="E214" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="215">
@@ -4286,16 +4286,16 @@
         <v>79</v>
       </c>
       <c r="B215" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C215" t="n">
-        <v>20248</v>
+        <v>664694</v>
       </c>
       <c r="D215" t="n">
-        <v>69383</v>
+        <v>2277675</v>
       </c>
       <c r="E215" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="216">
@@ -4303,16 +4303,16 @@
         <v>79</v>
       </c>
       <c r="B216" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C216" t="n">
-        <v>663576</v>
+        <v>20257</v>
       </c>
       <c r="D216" t="n">
-        <v>2273844</v>
+        <v>69414</v>
       </c>
       <c r="E216" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="217">
@@ -4323,13 +4323,13 @@
         <v>8</v>
       </c>
       <c r="C217" t="n">
-        <v>683824</v>
+        <v>684951</v>
       </c>
       <c r="D217" t="n">
-        <v>2343227</v>
+        <v>2347089</v>
       </c>
       <c r="E217" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="218">
@@ -4337,16 +4337,16 @@
         <v>80</v>
       </c>
       <c r="B218" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C218" t="n">
-        <v>694</v>
+        <v>19989</v>
       </c>
       <c r="D218" t="n">
-        <v>55114</v>
+        <v>1587436</v>
       </c>
       <c r="E218" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="219">
@@ -4354,16 +4354,16 @@
         <v>80</v>
       </c>
       <c r="B219" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C219" t="n">
-        <v>19932</v>
+        <v>694</v>
       </c>
       <c r="D219" t="n">
-        <v>1582910</v>
+        <v>55114</v>
       </c>
       <c r="E219" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="220">
@@ -4374,13 +4374,13 @@
         <v>8</v>
       </c>
       <c r="C220" t="n">
-        <v>20626</v>
+        <v>20683</v>
       </c>
       <c r="D220" t="n">
-        <v>1638024</v>
+        <v>1642551</v>
       </c>
       <c r="E220" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="221">
@@ -4391,13 +4391,13 @@
         <v>6</v>
       </c>
       <c r="C221" t="n">
-        <v>40112</v>
+        <v>40248</v>
       </c>
       <c r="D221" t="n">
-        <v>1670011</v>
+        <v>1675673</v>
       </c>
       <c r="E221" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="222">
@@ -4408,13 +4408,13 @@
         <v>7</v>
       </c>
       <c r="C222" t="n">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="D222" t="n">
-        <v>42383</v>
+        <v>42466</v>
       </c>
       <c r="E222" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="223">
@@ -4425,13 +4425,13 @@
         <v>8</v>
       </c>
       <c r="C223" t="n">
-        <v>41130</v>
+        <v>41268</v>
       </c>
       <c r="D223" t="n">
-        <v>1712394</v>
+        <v>1718140</v>
       </c>
       <c r="E223" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="224">
@@ -4442,13 +4442,13 @@
         <v>6</v>
       </c>
       <c r="C224" t="n">
-        <v>425913</v>
+        <v>426729</v>
       </c>
       <c r="D224" t="n">
-        <v>2235306</v>
+        <v>2239589</v>
       </c>
       <c r="E224" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="225">
@@ -4459,13 +4459,13 @@
         <v>7</v>
       </c>
       <c r="C225" t="n">
-        <v>11863</v>
+        <v>11875</v>
       </c>
       <c r="D225" t="n">
-        <v>62260</v>
+        <v>62323</v>
       </c>
       <c r="E225" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="226">
@@ -4476,13 +4476,13 @@
         <v>8</v>
       </c>
       <c r="C226" t="n">
-        <v>437776</v>
+        <v>438604</v>
       </c>
       <c r="D226" t="n">
-        <v>2297566</v>
+        <v>2301912</v>
       </c>
       <c r="E226" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="227">
@@ -4490,16 +4490,16 @@
         <v>83</v>
       </c>
       <c r="B227" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C227" t="n">
-        <v>2177</v>
+        <v>78584</v>
       </c>
       <c r="D227" t="n">
-        <v>52878</v>
+        <v>1908769</v>
       </c>
       <c r="E227" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="228">
@@ -4507,16 +4507,16 @@
         <v>83</v>
       </c>
       <c r="B228" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C228" t="n">
-        <v>78458</v>
+        <v>2177</v>
       </c>
       <c r="D228" t="n">
-        <v>1905708</v>
+        <v>52878</v>
       </c>
       <c r="E228" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="229">
@@ -4527,13 +4527,13 @@
         <v>8</v>
       </c>
       <c r="C229" t="n">
-        <v>80635</v>
+        <v>80761</v>
       </c>
       <c r="D229" t="n">
-        <v>1958586</v>
+        <v>1961647</v>
       </c>
       <c r="E229" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="230">
@@ -4544,13 +4544,13 @@
         <v>6</v>
       </c>
       <c r="C230" t="n">
-        <v>7783</v>
+        <v>7817</v>
       </c>
       <c r="D230" t="n">
-        <v>961576</v>
+        <v>965777</v>
       </c>
       <c r="E230" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="231">
@@ -4567,7 +4567,7 @@
         <v>10749</v>
       </c>
       <c r="E231" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="232">
@@ -4578,13 +4578,13 @@
         <v>8</v>
       </c>
       <c r="C232" t="n">
-        <v>7870</v>
+        <v>7904</v>
       </c>
       <c r="D232" t="n">
-        <v>972325</v>
+        <v>976526</v>
       </c>
       <c r="E232" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="233">
@@ -4595,13 +4595,13 @@
         <v>6</v>
       </c>
       <c r="C233" t="n">
-        <v>136142</v>
+        <v>136449</v>
       </c>
       <c r="D233" t="n">
-        <v>1998503</v>
+        <v>2003009</v>
       </c>
       <c r="E233" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="234">
@@ -4612,13 +4612,13 @@
         <v>7</v>
       </c>
       <c r="C234" t="n">
-        <v>3585</v>
+        <v>3587</v>
       </c>
       <c r="D234" t="n">
-        <v>52626</v>
+        <v>52656</v>
       </c>
       <c r="E234" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="235">
@@ -4629,13 +4629,13 @@
         <v>8</v>
       </c>
       <c r="C235" t="n">
-        <v>139727</v>
+        <v>140036</v>
       </c>
       <c r="D235" t="n">
-        <v>2051129</v>
+        <v>2055665</v>
       </c>
       <c r="E235" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="236">
@@ -4646,13 +4646,13 @@
         <v>6</v>
       </c>
       <c r="C236" t="n">
-        <v>285259</v>
+        <v>285731</v>
       </c>
       <c r="D236" t="n">
-        <v>1792639</v>
+        <v>1795605</v>
       </c>
       <c r="E236" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="237">
@@ -4663,13 +4663,13 @@
         <v>7</v>
       </c>
       <c r="C237" t="n">
-        <v>12148</v>
+        <v>12152</v>
       </c>
       <c r="D237" t="n">
-        <v>76341</v>
+        <v>76366</v>
       </c>
       <c r="E237" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="238">
@@ -4680,13 +4680,13 @@
         <v>8</v>
       </c>
       <c r="C238" t="n">
-        <v>297407</v>
+        <v>297883</v>
       </c>
       <c r="D238" t="n">
-        <v>1868980</v>
+        <v>1871971</v>
       </c>
       <c r="E238" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="239">
@@ -4697,13 +4697,13 @@
         <v>6</v>
       </c>
       <c r="C239" t="n">
-        <v>94544</v>
+        <v>94677</v>
       </c>
       <c r="D239" t="n">
-        <v>1550817</v>
+        <v>1552998</v>
       </c>
       <c r="E239" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="240">
@@ -4714,13 +4714,13 @@
         <v>7</v>
       </c>
       <c r="C240" t="n">
-        <v>2167</v>
+        <v>2168</v>
       </c>
       <c r="D240" t="n">
-        <v>35546</v>
+        <v>35562</v>
       </c>
       <c r="E240" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="241">
@@ -4731,13 +4731,13 @@
         <v>8</v>
       </c>
       <c r="C241" t="n">
-        <v>96711</v>
+        <v>96845</v>
       </c>
       <c r="D241" t="n">
-        <v>1586362</v>
+        <v>1588560</v>
       </c>
       <c r="E241" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="242">
@@ -4748,13 +4748,13 @@
         <v>6</v>
       </c>
       <c r="C242" t="n">
-        <v>105681</v>
+        <v>105898</v>
       </c>
       <c r="D242" t="n">
-        <v>2022796</v>
+        <v>2026950</v>
       </c>
       <c r="E242" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="243">
@@ -4771,7 +4771,7 @@
         <v>59030</v>
       </c>
       <c r="E243" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="244">
@@ -4782,13 +4782,13 @@
         <v>8</v>
       </c>
       <c r="C244" t="n">
-        <v>108765</v>
+        <v>108982</v>
       </c>
       <c r="D244" t="n">
-        <v>2081826</v>
+        <v>2085980</v>
       </c>
       <c r="E244" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="245">
@@ -4796,14 +4796,14 @@
         <v>89</v>
       </c>
       <c r="B245" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C245" t="n">
-        <v>35658</v>
+        <v>833320</v>
       </c>
       <c r="D245"/>
       <c r="E245" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="246">
@@ -4811,14 +4811,14 @@
         <v>89</v>
       </c>
       <c r="B246" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C246" t="n">
-        <v>831399</v>
+        <v>35678</v>
       </c>
       <c r="D246"/>
       <c r="E246" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="247">
@@ -4829,11 +4829,11 @@
         <v>8</v>
       </c>
       <c r="C247" t="n">
-        <v>867057</v>
+        <v>868998</v>
       </c>
       <c r="D247"/>
       <c r="E247" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="248">
@@ -4841,16 +4841,16 @@
         <v>90</v>
       </c>
       <c r="B248" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C248" t="n">
-        <v>2155</v>
+        <v>164572</v>
       </c>
       <c r="D248" t="n">
-        <v>28476</v>
+        <v>2174663</v>
       </c>
       <c r="E248" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="249">
@@ -4858,16 +4858,16 @@
         <v>90</v>
       </c>
       <c r="B249" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C249" t="n">
-        <v>164299</v>
+        <v>2155</v>
       </c>
       <c r="D249" t="n">
-        <v>2171056</v>
+        <v>28476</v>
       </c>
       <c r="E249" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="250">
@@ -4878,13 +4878,13 @@
         <v>8</v>
       </c>
       <c r="C250" t="n">
-        <v>166454</v>
+        <v>166727</v>
       </c>
       <c r="D250" t="n">
-        <v>2199532</v>
+        <v>2203140</v>
       </c>
       <c r="E250" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="251">
@@ -4892,16 +4892,16 @@
         <v>91</v>
       </c>
       <c r="B251" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C251" t="n">
-        <v>22066</v>
+        <v>1440299</v>
       </c>
       <c r="D251" t="n">
-        <v>60027</v>
+        <v>3918104</v>
       </c>
       <c r="E251" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="252">
@@ -4909,16 +4909,16 @@
         <v>91</v>
       </c>
       <c r="B252" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C252" t="n">
-        <v>1436411</v>
+        <v>22075</v>
       </c>
       <c r="D252" t="n">
-        <v>3907527</v>
+        <v>60052</v>
       </c>
       <c r="E252" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="253">
@@ -4929,13 +4929,13 @@
         <v>8</v>
       </c>
       <c r="C253" t="n">
-        <v>1458477</v>
+        <v>1462374</v>
       </c>
       <c r="D253" t="n">
-        <v>3967554</v>
+        <v>3978156</v>
       </c>
       <c r="E253" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="254">
@@ -4943,16 +4943,16 @@
         <v>92</v>
       </c>
       <c r="B254" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C254" t="n">
-        <v>107289</v>
+        <v>2893219</v>
       </c>
       <c r="D254" t="n">
-        <v>97199</v>
+        <v>2621116</v>
       </c>
       <c r="E254" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="255">
@@ -4960,16 +4960,16 @@
         <v>92</v>
       </c>
       <c r="B255" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C255" t="n">
-        <v>2883163</v>
+        <v>107386</v>
       </c>
       <c r="D255" t="n">
-        <v>2612005</v>
+        <v>97286</v>
       </c>
       <c r="E255" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="256">
@@ -4980,13 +4980,13 @@
         <v>8</v>
       </c>
       <c r="C256" t="n">
-        <v>2990452</v>
+        <v>3000605</v>
       </c>
       <c r="D256" t="n">
-        <v>2709204</v>
+        <v>2718402</v>
       </c>
       <c r="E256" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="257">
@@ -4997,13 +4997,13 @@
         <v>6</v>
       </c>
       <c r="C257" t="n">
-        <v>58016</v>
+        <v>58206</v>
       </c>
       <c r="D257" t="n">
-        <v>1725075</v>
+        <v>1730725</v>
       </c>
       <c r="E257" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="258">
@@ -5014,13 +5014,13 @@
         <v>7</v>
       </c>
       <c r="C258" t="n">
-        <v>1663</v>
+        <v>1664</v>
       </c>
       <c r="D258" t="n">
-        <v>49448</v>
+        <v>49478</v>
       </c>
       <c r="E258" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
     <row r="259">
@@ -5031,13 +5031,13 @@
         <v>8</v>
       </c>
       <c r="C259" t="n">
-        <v>59679</v>
+        <v>59870</v>
       </c>
       <c r="D259" t="n">
-        <v>1774524</v>
+        <v>1780203</v>
       </c>
       <c r="E259" s="1" t="n">
-        <v>44733.6235708333</v>
+        <v>44735.3826942409</v>
       </c>
     </row>
   </sheetData>

</xml_diff>